<commit_message>
Added all webex link
</commit_message>
<xml_diff>
--- a/Excel/Webex Dosen.xlsx
+++ b/Excel/Webex Dosen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Folder_apps\NGODING\Discord_bot\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E7A891-7D73-4162-944C-FF9576FBD38A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{499C5649-FD3E-4A5E-807C-8A0EFD626838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5865" yWindow="1575" windowWidth="17505" windowHeight="13905" xr2:uid="{09844CD0-0772-403D-951E-E5EC10EBBED1}"/>
+    <workbookView xWindow="240" yWindow="1635" windowWidth="17505" windowHeight="13905" xr2:uid="{09844CD0-0772-403D-951E-E5EC10EBBED1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>GUSSAN</t>
   </si>
@@ -48,19 +48,123 @@
   </si>
   <si>
     <t>Link</t>
+  </si>
+  <si>
+    <t>GUSMUL</t>
+  </si>
+  <si>
+    <t>GUSDE</t>
+  </si>
+  <si>
+    <t>MOGI</t>
+  </si>
+  <si>
+    <t>GUNGDE</t>
+  </si>
+  <si>
+    <t>HENDRA</t>
+  </si>
+  <si>
+    <t>EKA</t>
+  </si>
+  <si>
+    <t>https://universitas-udayana.webex.com/meet/arimogi</t>
+  </si>
+  <si>
+    <t>https://universitas-udayana.webex.com/meet/gungde</t>
+  </si>
+  <si>
+    <t>https://universitas-udayana.webex.com/meet/ibm.mahendra</t>
+  </si>
+  <si>
+    <t>https://universitas-udayana.webex.com/meet/eka.karyawati</t>
+  </si>
+  <si>
+    <t>https://universitas-udayana.webex.com/meet/dwidasmara</t>
+  </si>
+  <si>
+    <t>https://universitas-udayana.webex.com/meet/muliantara</t>
+  </si>
+  <si>
+    <t>ANOM</t>
+  </si>
+  <si>
+    <t>https://universitas-udayana.webex.com/meet/anom.cp</t>
+  </si>
+  <si>
+    <t>VIDA</t>
+  </si>
+  <si>
+    <t>https://universitas-udayana.webex.com/meet/vida</t>
+  </si>
+  <si>
+    <t>ASTUTI</t>
+  </si>
+  <si>
+    <t>https://universitas-udayana.webex.com/meet/lg.astuti</t>
+  </si>
+  <si>
+    <t>DAYU</t>
+  </si>
+  <si>
+    <t>https://universitas-udayana.webex.com/meet/idgsuwiprabayantiputra</t>
+  </si>
+  <si>
+    <t>COK</t>
+  </si>
+  <si>
+    <t>https://universitas-udayana.webex.com/meet/cokorda</t>
+  </si>
+  <si>
+    <t>SURYA</t>
+  </si>
+  <si>
+    <t>https://universitas-udayana.webex.com/meet/surya</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -71,7 +175,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -79,15 +183,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Hyperlink 2" xfId="4" xr:uid="{9DCDEA4F-E94E-4438-8C7C-1ADC12366780}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{10A798A6-449F-473E-ACB7-ABE6AFB8724B}"/>
+    <cellStyle name="Normal 2 2" xfId="2" xr:uid="{109005D1-913B-4943-9DCE-2F24B27C4014}"/>
+    <cellStyle name="Normal 4" xfId="1" xr:uid="{E5A7871E-05DB-40EE-BAC0-91FABD7DAF09}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -399,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E41EF8A4-DAAD-4AD3-9908-5A8C40BD0C86}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,7 +562,106 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{A7C19DF1-1CC8-4D1F-882B-0E84E3BB2162}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>